<commit_message>
Adicionado Log4j e TestNG com os casos de teste validos e invalidos
</commit_message>
<xml_diff>
--- a/produtosData.xlsx
+++ b/produtosData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\celso.silva\Cucumber\ProjetoLoja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C478889-3228-40B9-A4CD-9C940ABE444B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE79ADF4-ADCF-472E-9BD4-8B5033962899}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4F28670B-6503-4326-B193-0008A048BF3E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>Nome</t>
   </si>
@@ -51,7 +51,7 @@
     <t>PASS</t>
   </si>
   <si>
-    <t>NAO</t>
+    <t>Celular</t>
   </si>
 </sst>
 </file>
@@ -419,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0E2EB8E-17B2-44E2-AD63-5F7E96DD2E97}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,7 +449,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -458,6 +458,11 @@
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>